<commit_message>
ajout des emplacements des doc ap4
</commit_message>
<xml_diff>
--- a/public/doc/Tableau de synthese E4.xlsx
+++ b/public/doc/Tableau de synthese E4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaël BOISSON\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaël BOISSON\Desktop\Portfolio\public\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DCCFB5-43AF-4800-9547-DFFB757330BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF54E66-D851-4C9A-B2A4-8754C551F495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>N° candidat : 02244065459</t>
+  </si>
+  <si>
+    <t>01/11/2022 au 07/02/2023</t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -764,15 +767,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -806,44 +848,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1248,7 +1257,7 @@
   <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="73" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1261,56 +1270,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
@@ -1322,22 +1331,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1360,8 +1369,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="19" t="s">
         <v>14</v>
       </c>
@@ -1417,16 +1426,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1467,15 +1476,15 @@
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="14"/>
@@ -1517,20 +1526,20 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="22" t="s">
         <v>25</v>
       </c>
       <c r="I10"/>
@@ -1570,10 +1579,10 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="14"/>
@@ -1581,7 +1590,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="22" t="s">
         <v>25</v>
       </c>
       <c r="I11"/>
@@ -1621,15 +1630,15 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="22" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="14"/>
@@ -1672,19 +1681,19 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="15"/>
@@ -1725,21 +1734,21 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="47">
-        <v>44855</v>
+      <c r="B14" s="48" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="15"/>
@@ -1780,19 +1789,19 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="25">
         <v>44999</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="22" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="15"/>
@@ -1834,7 +1843,7 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -1968,16 +1977,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2330,16 +2339,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2377,14 +2386,14 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="14"/>
@@ -2790,11 +2799,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2802,6 +2806,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2813,15 +2822,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
@@ -2830,6 +2830,15 @@
     <TaxCatchAll xmlns="57e91659-be1d-4d29-8a34-37188ca8e23d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3056,20 +3065,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0BFF56-BE1D-4AD9-9F23-E461DD70F79B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE4E27C2-9E50-4B05-A279-A1A1A8E00469}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a54630e7-b857-4bdf-808b-f1da7c130004"/>
     <ds:schemaRef ds:uri="57e91659-be1d-4d29-8a34-37188ca8e23d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0BFF56-BE1D-4AD9-9F23-E461DD70F79B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>